<commit_message>
Upgraded speedtest-cli package to version 2.1.3 in requirements.txt Note: Version 2.1.2 is not working anymore
</commit_message>
<xml_diff>
--- a/speedtest_results.xlsx
+++ b/speedtest_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\Python\study\speedtest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45F15F18-C3AF-4D2D-87EF-9F456A135FFF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1915711A-09CB-406E-91FE-6DB34F37FF87}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{D0E09EAE-66B0-4CDD-81D0-596BD5A5C974}"/>
   </bookViews>
@@ -23,7 +23,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="23" r:id="rId4"/>
+    <pivotCache cacheId="24" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -306,37 +306,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="30">
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" indent="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" indent="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" indent="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" indent="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" indent="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" indent="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" indent="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" indent="0"/>
-    </dxf>
+  <dxfs count="20">
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -434,7 +404,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[resultados_speedtest.xlsx]DASH!Tabela dinâmica1</c:name>
+    <c:name>[speedtest_results.xlsx]DASH!Tabela dinâmica1</c:name>
     <c:fmtId val="32"/>
   </c:pivotSource>
   <c:chart>
@@ -2786,7 +2756,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{88866C90-9F69-4D66-A565-DE9D6AEB267A}" name="Tabela dinâmica1" cacheId="23" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="41" rowHeaderCaption=".">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{88866C90-9F69-4D66-A565-DE9D6AEB267A}" name="Tabela dinâmica1" cacheId="24" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="41" rowHeaderCaption=".">
   <location ref="B4:D10" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="10">
     <pivotField axis="axisRow" numFmtId="22" showAll="0">
@@ -3238,7 +3208,7 @@
     <dataField name="Up Speed" fld="2" subtotal="average" baseField="9" baseItem="1" numFmtId="165"/>
   </dataFields>
   <formats count="10">
-    <format dxfId="29">
+    <format dxfId="19">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="2" selected="0">
@@ -3248,7 +3218,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="28">
+    <format dxfId="18">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="2">
@@ -3258,16 +3228,16 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="27">
+    <format dxfId="17">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="26">
+    <format dxfId="16">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="25">
+    <format dxfId="15">
       <pivotArea field="9" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="24">
+    <format dxfId="14">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="9" count="1">
@@ -3276,10 +3246,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="23">
+    <format dxfId="13">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="22">
+    <format dxfId="12">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="8" count="1">
@@ -3291,7 +3261,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="21">
+    <format dxfId="11">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="3">
           <reference field="0" count="1">
@@ -3306,7 +3276,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="20">
+    <format dxfId="10">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="2">
@@ -3511,17 +3481,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C2979AF4-7875-480A-B86A-816D31E2F07D}" name="database" displayName="database" ref="A1:H41" tableType="queryTable" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C2979AF4-7875-480A-B86A-816D31E2F07D}" name="database" displayName="database" ref="A1:H41" tableType="queryTable" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
   <autoFilter ref="A1:H41" xr:uid="{409ABEB7-3B99-42FD-BF5F-F12B18660826}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{F0B9D545-A21A-4D48-A4FA-DEE35B4F208E}" uniqueName="1" name="timestamp" queryTableFieldId="1" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{E81261FA-CB5B-46A4-A233-B022E0D30DF1}" uniqueName="2" name="download_speed_Mbps" queryTableFieldId="2" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{C35FD570-55EE-4D85-8316-D6E86B1DA4BB}" uniqueName="3" name="upload_speed_Mbps" queryTableFieldId="3" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{50532527-8F55-4DA3-AF36-27158C12ACD2}" uniqueName="4" name="ping_ms" queryTableFieldId="4" dataDxfId="14"/>
-    <tableColumn id="5" xr3:uid="{1F42D213-2FD8-492A-BF12-C035D9121E21}" uniqueName="5" name="provider" queryTableFieldId="5" dataDxfId="13"/>
-    <tableColumn id="6" xr3:uid="{A4462B30-9E9F-4492-BA46-C7219F166312}" uniqueName="6" name="ip" queryTableFieldId="6" dataDxfId="12"/>
-    <tableColumn id="7" xr3:uid="{8D23EBC0-5F3C-49EA-A2C2-384388DDE9BF}" uniqueName="7" name="mb_sent" queryTableFieldId="7" dataDxfId="11"/>
-    <tableColumn id="8" xr3:uid="{1B2683FB-045F-42A8-A5CA-D0D7EA7ED4F2}" uniqueName="8" name="mb_received" queryTableFieldId="8" dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{F0B9D545-A21A-4D48-A4FA-DEE35B4F208E}" uniqueName="1" name="timestamp" queryTableFieldId="1" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{E81261FA-CB5B-46A4-A233-B022E0D30DF1}" uniqueName="2" name="download_speed_Mbps" queryTableFieldId="2" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{C35FD570-55EE-4D85-8316-D6E86B1DA4BB}" uniqueName="3" name="upload_speed_Mbps" queryTableFieldId="3" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{50532527-8F55-4DA3-AF36-27158C12ACD2}" uniqueName="4" name="ping_ms" queryTableFieldId="4" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{1F42D213-2FD8-492A-BF12-C035D9121E21}" uniqueName="5" name="provider" queryTableFieldId="5" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{A4462B30-9E9F-4492-BA46-C7219F166312}" uniqueName="6" name="ip" queryTableFieldId="6" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{8D23EBC0-5F3C-49EA-A2C2-384388DDE9BF}" uniqueName="7" name="mb_sent" queryTableFieldId="7" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{1B2683FB-045F-42A8-A5CA-D0D7EA7ED4F2}" uniqueName="8" name="mb_received" queryTableFieldId="8" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>

</xml_diff>